<commit_message>
Aprimoramento, correção de falha na modelagem
</commit_message>
<xml_diff>
--- a/Modelagem - Locadora/Excel.xlsx
+++ b/Modelagem - Locadora/Excel.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20348"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D13AAF17-36ED-4009-9B08-D79BBD50E9DB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -136,7 +135,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -254,24 +253,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -291,6 +272,24 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -570,11 +569,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9:G13"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -582,376 +581,376 @@
     <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
       <c r="E2" s="1"/>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="15"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="9"/>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B3" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="11" t="s">
+      <c r="B3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>3</v>
       </c>
       <c r="E3" s="2"/>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="H3" s="10" t="s">
+      <c r="G3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B4" s="6">
+        <v>1</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="6">
+        <v>1</v>
+      </c>
+      <c r="G4" s="6">
+        <v>3</v>
+      </c>
+      <c r="H4" s="6">
+        <v>3</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B5" s="6">
+        <v>2</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="F5" s="6">
+        <v>2</v>
+      </c>
+      <c r="G5" s="6">
+        <v>3</v>
+      </c>
+      <c r="H5" s="6">
+        <v>2</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B6" s="6">
+        <v>3</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="6">
+        <v>3</v>
+      </c>
+      <c r="G6" s="6">
+        <v>3</v>
+      </c>
+      <c r="H6" s="6">
+        <v>1</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B8" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="17"/>
+      <c r="D8" s="18"/>
+      <c r="F8" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="9"/>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B9" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B10" s="6">
+        <v>1</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="6">
+        <v>123456789</v>
+      </c>
+      <c r="F10" s="6">
+        <v>1</v>
+      </c>
+      <c r="G10" s="6">
+        <v>3</v>
+      </c>
+      <c r="H10" s="6">
+        <v>3</v>
+      </c>
+      <c r="I10" s="11">
+        <v>43811</v>
+      </c>
+      <c r="J10" s="12">
+        <v>43811</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B11" s="6">
+        <v>2</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="6">
+        <v>987654232</v>
+      </c>
+      <c r="F11" s="6">
+        <v>2</v>
+      </c>
+      <c r="G11" s="6">
+        <v>2</v>
+      </c>
+      <c r="H11" s="6">
+        <v>3</v>
+      </c>
+      <c r="I11" s="11">
+        <v>43780</v>
+      </c>
+      <c r="J11" s="12">
+        <v>43694</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B12" s="6">
+        <v>3</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="6">
+        <v>123321876</v>
+      </c>
+      <c r="F12" s="6">
+        <v>3</v>
+      </c>
+      <c r="G12" s="6">
+        <v>4</v>
+      </c>
+      <c r="H12" s="6">
+        <v>1</v>
+      </c>
+      <c r="I12" s="11">
+        <v>43717</v>
+      </c>
+      <c r="J12" s="12">
+        <v>43477</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B13" s="6">
+        <v>4</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="6">
+        <v>345789234</v>
+      </c>
+      <c r="F13" s="6">
+        <v>4</v>
+      </c>
+      <c r="G13" s="6">
+        <v>1</v>
+      </c>
+      <c r="H13" s="6">
+        <v>2</v>
+      </c>
+      <c r="I13" s="11">
+        <v>43748</v>
+      </c>
+      <c r="J13" s="12">
+        <v>43811</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="E15" s="8"/>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B16" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="13"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B4" s="12">
-        <v>1</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="12">
-        <v>1</v>
-      </c>
-      <c r="G4" s="12">
-        <v>3</v>
-      </c>
-      <c r="H4" s="12">
-        <v>3</v>
-      </c>
-      <c r="I4" s="12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="12">
-        <v>2</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="12">
-        <v>2</v>
-      </c>
-      <c r="G5" s="12">
-        <v>3</v>
-      </c>
-      <c r="H5" s="12">
-        <v>2</v>
-      </c>
-      <c r="I5" s="12" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="12">
-        <v>3</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="12">
-        <v>3</v>
-      </c>
-      <c r="G6" s="12">
-        <v>3</v>
-      </c>
-      <c r="H6" s="12">
-        <v>1</v>
-      </c>
-      <c r="I6" s="12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="9"/>
-      <c r="F8" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="F9" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="I9" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="J9" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="K9" s="10" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="12">
-        <v>1</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="12">
-        <v>123456789</v>
-      </c>
-      <c r="F10" s="12">
-        <v>1</v>
-      </c>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12">
-        <v>3</v>
-      </c>
-      <c r="I10" s="12">
-        <v>3</v>
-      </c>
-      <c r="J10" s="17">
-        <v>43811</v>
-      </c>
-      <c r="K10" s="18">
-        <v>43811</v>
-      </c>
-    </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="12">
-        <v>2</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" s="12">
-        <v>987654232</v>
-      </c>
-      <c r="F11" s="12">
-        <v>2</v>
-      </c>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12">
-        <v>2</v>
-      </c>
-      <c r="I11" s="12">
-        <v>3</v>
-      </c>
-      <c r="J11" s="17">
-        <v>43780</v>
-      </c>
-      <c r="K11" s="18">
-        <v>43694</v>
-      </c>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="12">
-        <v>3</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" s="12">
-        <v>123321876</v>
-      </c>
-      <c r="F12" s="12">
-        <v>3</v>
-      </c>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12">
-        <v>4</v>
-      </c>
-      <c r="I12" s="12">
-        <v>1</v>
-      </c>
-      <c r="J12" s="17">
-        <v>43717</v>
-      </c>
-      <c r="K12" s="18">
-        <v>43477</v>
-      </c>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="12">
-        <v>4</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" s="12">
-        <v>345789234</v>
-      </c>
-      <c r="F13" s="12">
-        <v>4</v>
-      </c>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12">
-        <v>1</v>
-      </c>
-      <c r="I13" s="12">
-        <v>2</v>
-      </c>
-      <c r="J13" s="17">
-        <v>43748</v>
-      </c>
-      <c r="K13" s="18">
-        <v>43811</v>
-      </c>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="E15" s="14"/>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B16" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G16" s="6"/>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="10" t="s">
+      <c r="C17" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H17" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E17" s="3"/>
-      <c r="F17" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="G17" s="10" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="12">
-        <v>1</v>
-      </c>
-      <c r="C18" s="12" t="s">
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" s="6">
+        <v>1</v>
+      </c>
+      <c r="C18" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D18" s="12">
-        <v>2</v>
-      </c>
+      <c r="D18" s="3"/>
       <c r="E18" s="3"/>
-      <c r="F18" s="12">
-        <v>1</v>
-      </c>
-      <c r="G18" s="12" t="s">
+      <c r="F18" s="6">
+        <v>1</v>
+      </c>
+      <c r="G18" s="6" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="12">
-        <v>2</v>
-      </c>
-      <c r="C19" s="12" t="s">
+      <c r="H18" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19" s="6">
+        <v>2</v>
+      </c>
+      <c r="C19" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D19" s="12">
-        <v>3</v>
-      </c>
+      <c r="D19" s="3"/>
       <c r="E19" s="3"/>
-      <c r="F19" s="12">
-        <v>2</v>
-      </c>
-      <c r="G19" s="12" t="s">
+      <c r="F19" s="6">
+        <v>2</v>
+      </c>
+      <c r="G19" s="6" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="12">
-        <v>3</v>
-      </c>
-      <c r="C20" s="12" t="s">
+      <c r="H19" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="6">
+        <v>3</v>
+      </c>
+      <c r="C20" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D20" s="12">
-        <v>1</v>
-      </c>
+      <c r="D20" s="3"/>
       <c r="E20" s="3"/>
-      <c r="F20" s="12">
-        <v>3</v>
-      </c>
-      <c r="G20" s="12" t="s">
+      <c r="F20" s="6">
+        <v>3</v>
+      </c>
+      <c r="G20" s="6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="E21" s="14"/>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="E22" s="16"/>
+      <c r="H20" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E21" s="8"/>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E22" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="F8:K8"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="F16:G16"/>
     <mergeCell ref="F2:I2"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="F8:J8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>